<commit_message>
clone and pull from branch
</commit_message>
<xml_diff>
--- a/Angular/input.xlsx
+++ b/Angular/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dotnet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Clone_Path</t>
   </si>
@@ -52,16 +52,22 @@
     <t>D:\\Backup\\FileNa</t>
   </si>
   <si>
-    <t>I:\\PetmatrixDevopsClone</t>
-  </si>
-  <si>
-    <t>I:\\PetmatrixDevopsClone\\petmatrix-backend-kku\\PetMatrix.API\\bin\\Release\\netcoreapp2.1\\publish</t>
-  </si>
-  <si>
-    <t>I:\\PetMatrixDevops\\PetmatrixBackend</t>
-  </si>
-  <si>
-    <t>X:\\PetMatrixDevopsBackup\\second</t>
+    <t>D:\\PetmatrixDevopsClone</t>
+  </si>
+  <si>
+    <t>D:\\PetMatrixDevops\\PetmatrixBackend</t>
+  </si>
+  <si>
+    <t>D:\\PetMatrixDevopsBackup\\second</t>
+  </si>
+  <si>
+    <t>D:\\PetmatrixDevopsClone\\petmatrix-backend-kku\\PetMatrix.API\\bin\\Debug\\netcoreapp2.1\\publish</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>release</t>
   </si>
 </sst>
 </file>
@@ -393,13 +399,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.7109375" customWidth="1"/>
+    <col min="1" max="1" width="69.5703125" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="3" width="99.140625" customWidth="1"/>
     <col min="4" max="4" width="47.140625" customWidth="1"/>
@@ -423,7 +429,9 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -433,13 +441,16 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
+      <c r="F2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -453,10 +464,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +479,7 @@
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -484,8 +495,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -500,6 +514,9 @@
       </c>
       <c r="E2" t="s">
         <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>